<commit_message>
config renames and setup
</commit_message>
<xml_diff>
--- a/crated_models.xlsx
+++ b/crated_models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\PCGClassification\PCGTransformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18CD6D3-00D6-4ADE-9D93-B687853B855A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A3F405-CD68-4E66-80F6-6AFBA9581ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27900" yWindow="2235" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>Dataset</t>
   </si>
@@ -83,9 +83,6 @@
     <t>2022 fix kNN recall optimized</t>
   </si>
   <si>
-    <t>Probleme, neu optim</t>
-  </si>
-  <si>
     <t>Vergleiche</t>
   </si>
   <si>
@@ -98,37 +95,76 @@
     <t>kNN vs Linear</t>
   </si>
   <si>
-    <t>Wird optimiert</t>
-  </si>
-  <si>
-    <t>Entnehmen aus run</t>
-  </si>
-  <si>
-    <t>Train</t>
-  </si>
-  <si>
-    <t>Optim Nacht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">setted </t>
-  </si>
-  <si>
     <t>Ready</t>
   </si>
   <si>
     <t>When</t>
   </si>
   <si>
-    <t>Mix optims</t>
-  </si>
-  <si>
-    <t>Known optim</t>
-  </si>
-  <si>
     <t>Parameter source</t>
   </si>
   <si>
-    <t>knownOptim Prov.</t>
+    <t>Nacht 2</t>
+  </si>
+  <si>
+    <t>ready</t>
+  </si>
+  <si>
+    <t>2024-09-19_01-01-49_2016_fixed_cnn_finalrun</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>0.8648</t>
+  </si>
+  <si>
+    <t>2024-09-18_23-40-18_2016_fixed_beats_knn_finalrun</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>2024-09-19_00-14-00_2022_fixed_beats_knn_finalrun</t>
+  </si>
+  <si>
+    <t>0.6761</t>
+  </si>
+  <si>
+    <t>schlechte konsistenz, recall</t>
+  </si>
+  <si>
+    <t>To v2</t>
+  </si>
+  <si>
+    <t>Instabil</t>
+  </si>
+  <si>
+    <t>0.74</t>
+  </si>
+  <si>
+    <t>Instabil, Große STD</t>
+  </si>
+  <si>
+    <t>0.63</t>
+  </si>
+  <si>
+    <t>Schlecht Precision, Instabil</t>
+  </si>
+  <si>
+    <t>2024-09-19_00-46-46_2022_cycles_beats_knn_finalrun</t>
+  </si>
+  <si>
+    <t>2024-09-19_10-33-10_2022_fixed_cnn_finalrun</t>
+  </si>
+  <si>
+    <t>Kein Extra mehr</t>
+  </si>
+  <si>
+    <t>Weniger k</t>
+  </si>
+  <si>
+    <t>Spalte1</t>
   </si>
 </sst>
 </file>
@@ -150,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,13 +231,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="1" tint="0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -353,14 +395,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="19">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -486,6 +537,46 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -632,44 +723,44 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -704,19 +795,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{041AAF87-DAC6-4C06-B462-0F1CABFA1C18}" name="Tabelle1" displayName="Tabelle1" ref="B2:K17" headerRowDxfId="16" totalsRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14">
-  <autoFilter ref="B2:K17" xr:uid="{041AAF87-DAC6-4C06-B462-0F1CABFA1C18}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{F0DBBACC-A7D2-4CB3-B559-DE6548265725}" name="Dataset" totalsRowLabel="Ergebnis" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{56311A03-4E07-486F-A31C-8EA512B85502}" name="Chunks" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{7032849B-E28D-4D83-B6F7-C69E8398D0DE}" name="Method" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{D5C25D98-A7CF-4652-BBB2-7DDE6C26DB6C}" name="Sub-Method" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{EC90CC1B-CF67-4507-B97D-15685C412955}" name="Extra" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{B4033F45-D270-49BF-9B80-A3545CC2C66A}" name="Name" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{3AE4ABBF-83BC-4E4A-AF65-E18FA69F532E}" name="NMCC" totalsRowFunction="count" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{E0C851D3-B51A-456E-93BA-E3CBACF1FC16}" name="When" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{7E6309B4-9A57-4506-BC13-779938A13446}" name="Ready" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{A328F3C8-DA53-4914-9A3D-FE9A4FE9AFF0}" name="Parameter source" dataDxfId="1" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{041AAF87-DAC6-4C06-B462-0F1CABFA1C18}" name="Tabelle1" displayName="Tabelle1" ref="B2:L17" headerRowDxfId="18" totalsRowDxfId="15" headerRowBorderDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="B2:L17" xr:uid="{041AAF87-DAC6-4C06-B462-0F1CABFA1C18}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{F0DBBACC-A7D2-4CB3-B559-DE6548265725}" name="Dataset" totalsRowLabel="Ergebnis" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{56311A03-4E07-486F-A31C-8EA512B85502}" name="Chunks" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{7032849B-E28D-4D83-B6F7-C69E8398D0DE}" name="Method" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{D5C25D98-A7CF-4652-BBB2-7DDE6C26DB6C}" name="Sub-Method" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{EC90CC1B-CF67-4507-B97D-15685C412955}" name="Extra" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{B4033F45-D270-49BF-9B80-A3545CC2C66A}" name="Name" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{3AE4ABBF-83BC-4E4A-AF65-E18FA69F532E}" name="NMCC" totalsRowFunction="count" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{E0C851D3-B51A-456E-93BA-E3CBACF1FC16}" name="When" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{7E6309B4-9A57-4506-BC13-779938A13446}" name="Ready" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{A328F3C8-DA53-4914-9A3D-FE9A4FE9AFF0}" name="Parameter source" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{6C754B66-97BD-4666-8372-3F7558AD15F1}" name="Spalte1" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -985,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K26"/>
+  <dimension ref="A2:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,12 +1090,14 @@
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1026,16 +1120,19 @@
         <v>4</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="10">
         <v>2016</v>
       </c>
@@ -1046,44 +1143,44 @@
         <v>8</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
+      <c r="H3" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="28"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="23">
         <v>2016</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G4" s="24"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
         <v>2016</v>
       </c>
@@ -1096,18 +1193,20 @@
       <c r="E5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>2022</v>
       </c>
@@ -1119,19 +1218,20 @@
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G6" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="11">
         <v>2022</v>
       </c>
@@ -1144,22 +1244,19 @@
       <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="23" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="31"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>2022</v>
       </c>
@@ -1173,17 +1270,28 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>2022</v>
       </c>
@@ -1195,41 +1303,43 @@
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="11">
+      <c r="G9" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="29"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="23">
         <v>2022</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G10" s="24"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
         <v>2022</v>
       </c>
@@ -1242,18 +1352,22 @@
       <c r="E11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="G11" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="29"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1264,8 +1378,9 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1276,8 +1391,9 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1288,8 +1404,9 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
@@ -1302,8 +1419,9 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1314,8 +1432,9 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -1326,8 +1445,9 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="8"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>2016</v>
       </c>
@@ -1338,10 +1458,10 @@
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>2016</v>
       </c>
@@ -1355,10 +1475,10 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>2022</v>
       </c>
@@ -1369,10 +1489,10 @@
         <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>2022</v>
       </c>
@@ -1386,10 +1506,10 @@
         <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="18">
         <v>2022</v>
       </c>
@@ -1403,7 +1523,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>2022</v>
       </c>
@@ -1414,7 +1534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="18">
         <v>2022</v>
       </c>
@@ -1431,8 +1551,9 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>